<commit_message>
Fix ablation study visualization arrow and remove deprecated evaluation files
</commit_message>
<xml_diff>
--- a/results_claude_3.5/blind_evaluation_scoring_sheet_CLAUDE35.xlsx
+++ b/results_claude_3.5/blind_evaluation_scoring_sheet_CLAUDE35.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Specialist RAG vs Generalist RAG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Specialist RAG vs Generalist RAG\results_claude_3.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96BE20B-F804-4AFE-A7A9-D6B0A51B20D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14A8F1-7A9B-459C-A159-7DAE04E444DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>Question_ID</t>
   </si>
@@ -431,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -442,9 +442,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,14 +746,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="166.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="166.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="255.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.54296875" customWidth="1"/>
@@ -797,7 +794,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
@@ -826,7 +823,7 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
@@ -855,7 +852,7 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
@@ -884,7 +881,7 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
@@ -896,7 +893,7 @@
       <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>4</v>
       </c>
       <c r="G5">
@@ -913,7 +910,7 @@
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
       <c r="C6" t="s">
@@ -925,7 +922,7 @@
       <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6">
         <v>4</v>
       </c>
       <c r="G6">
@@ -942,7 +939,7 @@
       <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
@@ -954,7 +951,7 @@
       <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
@@ -971,7 +968,7 @@
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>35</v>
       </c>
       <c r="C8" t="s">
@@ -983,7 +980,7 @@
       <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
         <v>5</v>
       </c>
       <c r="G8">
@@ -1000,7 +997,7 @@
       <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>39</v>
       </c>
       <c r="C9" t="s">
@@ -1012,7 +1009,7 @@
       <c r="E9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9">
         <v>5</v>
       </c>
       <c r="G9">
@@ -1029,7 +1026,7 @@
       <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
       <c r="C10" t="s">
@@ -1041,13 +1038,16 @@
       <c r="E10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10">
         <v>5</v>
       </c>
       <c r="G10">
         <v>5</v>
       </c>
       <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>47</v>
       </c>
       <c r="C11" t="s">
@@ -1067,7 +1067,7 @@
       <c r="E11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11">
         <v>5</v>
       </c>
       <c r="G11">

</xml_diff>